<commit_message>
Added measurements on 4th of June
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/measurements.xlsx
+++ b/verilog/hardware/processor/source/measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\f-of-e-tools\verilog\hardware\processor\source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF78BF1-F788-4846-AACB-257ED16CFCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB8FF9F-0414-C24F-9CAA-FB3EC4CC95D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31400" windowHeight="15840" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>USE_CORRELATING</t>
   </si>
@@ -132,10 +132,13 @@
     <t>Proposal 1 + Adder</t>
   </si>
   <si>
-    <t>cache 1 word</t>
-  </si>
-  <si>
     <t>clock frequency (Hz)</t>
+  </si>
+  <si>
+    <t>Proposal 1 + ANDXOR</t>
+  </si>
+  <si>
+    <t>Cache 1 word</t>
   </si>
 </sst>
 </file>
@@ -210,7 +213,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,32 +525,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5514D7BD-1B29-5548-99C9-D3A14905CC46}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="62.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="4"/>
-    <col min="3" max="3" width="17.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="31.875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.875" style="4"/>
+    <col min="3" max="3" width="17.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
     <col min="7" max="7" width="11" style="3"/>
-    <col min="8" max="8" width="18.125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" style="3" customWidth="1"/>
     <col min="9" max="9" width="17" style="3" customWidth="1"/>
     <col min="10" max="10" width="11" style="3"/>
     <col min="11" max="11" width="22" style="3" customWidth="1"/>
     <col min="12" max="14" width="11" style="3"/>
-    <col min="15" max="15" width="19.375" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="17.83203125" style="3" customWidth="1"/>
     <col min="17" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
       <c r="D1" s="6" t="s">
         <v>18</v>
@@ -567,10 +570,10 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
@@ -610,7 +613,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -627,19 +630,19 @@
         <v>3238</v>
       </c>
       <c r="G4" s="3">
-        <f>$B4/(E4*C$31)</f>
+        <f>$B4/(E4*C$32)</f>
         <v>2.9847182425978982</v>
       </c>
       <c r="I4" s="3">
-        <f>D4/E4/192000*1000000000</f>
+        <f t="shared" ref="I4:I19" si="0">D4/E4/192000*1000000000</f>
         <v>2.0555505810251513</v>
       </c>
       <c r="N4" s="3" t="e">
-        <f>$B4/(L4*J$31)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B4/(L4*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -647,7 +650,7 @@
         <v>12000000</v>
       </c>
       <c r="D5" s="3">
-        <v>7.58203E-3</v>
+        <v>7.8554799999999998E-3</v>
       </c>
       <c r="E5" s="3">
         <v>20.95</v>
@@ -656,28 +659,31 @@
         <v>3238</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G20" si="0">$B5/(E5*C$31)</f>
+        <f>$B5/(E5*C$32)</f>
         <v>2.9832935560859188</v>
       </c>
       <c r="H5" s="3">
         <v>12.56</v>
       </c>
       <c r="I5" s="3">
-        <f>D5/E5/192000*1000000000</f>
-        <v>1.88495177008751</v>
+        <f t="shared" si="0"/>
+        <v>1.9529335719968179</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.055913E-2</v>
       </c>
       <c r="L5" s="3">
         <v>0.99099999999999999</v>
       </c>
       <c r="N5" s="3" t="e">
-        <f t="shared" ref="N5:N20" si="1">$B5/(L5*J$31)</f>
+        <f>$B5/(L5*J$32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="3">
         <v>12.26</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -694,19 +700,19 @@
         <v>3270</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="0"/>
+        <f>$B6/(E6*C$32)</f>
         <v>2.9861442904921165</v>
       </c>
       <c r="I6" s="3">
-        <f>D6/E6/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>2.1046096114030894</v>
       </c>
       <c r="N6" s="3" t="e">
-        <f>$B6/(L18*J$31)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B6/(L18*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -723,19 +729,19 @@
         <v>3270</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="0"/>
+        <f>$B7/(E7*C$32)</f>
         <v>2.979027645376549</v>
       </c>
       <c r="I7" s="3">
-        <f>D7/E7/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>1.9866043056879568</v>
       </c>
       <c r="N7" s="3" t="e">
-        <f>$B7/(L19*J$31)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B7/(L19*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -752,19 +758,19 @@
         <v>3247</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="0"/>
+        <f>$B8/(E8*C$32)</f>
         <v>2.9961649089165867</v>
       </c>
       <c r="I8" s="3">
-        <f>D8/E8/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>2.023709651645893</v>
       </c>
       <c r="N8" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B8/(L8*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -781,19 +787,19 @@
         <v>3222</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="0"/>
+        <f>$B9/(E9*C$32)</f>
         <v>3.0193236714975846</v>
       </c>
       <c r="I9" s="3">
-        <f>D9/E9/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>2.0343246779388084</v>
       </c>
       <c r="N9" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B9/(L9*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -810,42 +816,45 @@
         <v>3180</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="0"/>
+        <f>$B10/(E10*C$32)</f>
         <v>2.987571701720841</v>
       </c>
       <c r="I10" s="3">
-        <f>D10/E10/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>2.2026669056724026</v>
       </c>
       <c r="N10" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B10/(L10*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="4">
         <v>6000000</v>
       </c>
+      <c r="D11" s="3">
+        <v>4.4683600000000002E-3</v>
+      </c>
       <c r="F11" s="4">
         <v>3238</v>
       </c>
       <c r="G11" s="3" t="e">
-        <f t="shared" si="0"/>
+        <f>$B11/(E11*C$32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" s="3" t="e">
-        <f>D11/E11/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B11/(L11*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -862,19 +871,19 @@
         <v>3216</v>
       </c>
       <c r="G12" s="3">
-        <f t="shared" si="0"/>
+        <f>$B12/(E12*C$32)</f>
         <v>2.987571701720841</v>
       </c>
       <c r="I12" s="3">
-        <f>D12/E12/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>1.929941443594646</v>
       </c>
       <c r="N12" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B12/(L12*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -891,19 +900,19 @@
         <v>3238</v>
       </c>
       <c r="G13" s="3">
-        <f t="shared" si="0"/>
+        <f>$B13/(E13*C$32)</f>
         <v>2.9861442904921165</v>
       </c>
       <c r="I13" s="3">
-        <f>D13/E13/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>2.0572941551202417</v>
       </c>
       <c r="N13" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B13/(L13*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -914,19 +923,19 @@
         <v>3238</v>
       </c>
       <c r="G14" s="3" t="e">
-        <f t="shared" si="0"/>
+        <f>$B14/(E14*C$32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I14" s="3" t="e">
-        <f>D14/E14/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B14/(L14*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -943,19 +952,19 @@
         <v>3246</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" si="0"/>
+        <f>$B15/(E15*C$32)</f>
         <v>2.9932950191570882</v>
       </c>
       <c r="I15" s="3">
-        <f>D15/E15/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>4.3402478448275854</v>
       </c>
       <c r="N15" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <f>$B15/(L15*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -972,19 +981,19 @@
         <v>3238</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="0"/>
+        <f>$B16/(E16*C$32)</f>
         <v>2.9932950191570882</v>
       </c>
       <c r="I16" s="3">
-        <f>D16/E16/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>749.04214559386992</v>
       </c>
       <c r="N16" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+        <f>$B16/(L16*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -995,25 +1004,28 @@
         <v>1.1715339999999999E-2</v>
       </c>
       <c r="G17" s="3" t="e">
-        <f t="shared" si="0"/>
+        <f>$B17/(E17*C$32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I17" s="3" t="e">
-        <f>D17/E17/192000*1000000000</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N17" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+        <f>$B17/(L17*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="4">
         <v>12000000</v>
       </c>
+      <c r="D18" s="3">
+        <v>7.46066E-3</v>
+      </c>
       <c r="E18" s="3">
         <v>20.92</v>
       </c>
@@ -1021,15 +1033,18 @@
         <v>3252</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="0"/>
+        <f>$B18/(E18*C$32)</f>
         <v>2.987571701720841</v>
       </c>
       <c r="H18" s="3">
         <v>12.13</v>
       </c>
       <c r="I18" s="3">
-        <f>D18/E18/192000*1000000000</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.8574380576800509</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1.072027E-2</v>
       </c>
       <c r="L18" s="3">
         <v>0.98699999999999999</v>
@@ -1038,20 +1053,23 @@
         <v>4818</v>
       </c>
       <c r="N18" s="3" t="e">
-        <f>$B18/(#REF!*J$31)</f>
+        <f>$B18/(#REF!*J$32)</f>
         <v>#REF!</v>
       </c>
       <c r="O18" s="3">
         <v>13.94</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="4">
         <v>12000000</v>
       </c>
+      <c r="D19" s="3">
+        <v>7.84551E-3</v>
+      </c>
       <c r="E19" s="3">
         <v>20.95</v>
       </c>
@@ -1059,15 +1077,18 @@
         <v>3190</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="0"/>
+        <f>$B19/(E19*C$32)</f>
         <v>2.9832935560859188</v>
       </c>
       <c r="H19" s="3">
         <v>13.34</v>
       </c>
       <c r="I19" s="3">
-        <f>D19/E19/192000*1000000000</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1.9504549522673031</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1.102446E-2</v>
       </c>
       <c r="L19" s="3">
         <v>0.98599999999999999</v>
@@ -1076,72 +1097,86 @@
         <v>4753</v>
       </c>
       <c r="N19" s="3" t="e">
-        <f>$B19/(#REF!*J$31)</f>
+        <f>$B19/(#REF!*J$32)</f>
         <v>#REF!</v>
       </c>
       <c r="O19" s="3">
         <v>13.09</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B20" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="D20" s="3">
+        <v>8.1435699999999993E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="4">
         <v>6000000</v>
       </c>
-      <c r="E20" s="3">
+      <c r="D21" s="3">
+        <v>4.6831299999999998E-3</v>
+      </c>
+      <c r="E21" s="3">
         <v>10.73</v>
       </c>
-      <c r="G20" s="3">
-        <f t="shared" si="0"/>
+      <c r="G21" s="3">
+        <f>$B21/(E21*C$32)</f>
         <v>2.9123951537744643</v>
       </c>
-      <c r="N20" s="3" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="N21" s="3" t="e">
+        <f>$B21/(L21*J$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C32" s="3">
         <v>192000</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D37" s="3" t="s">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D38" s="3" t="s">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" s="3" t="s">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" s="3" t="s">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D41" s="3" t="s">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D42" s="3" t="s">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D43" s="3" t="s">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1150,8 +1185,8 @@
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="K1:P1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F4:F20">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="F4:F21">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1162,8 +1197,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G20">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="G4:G21">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1174,8 +1209,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H20">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="H4:H21">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1186,8 +1221,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I20">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="I4:I21">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1198,8 +1233,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D20">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D4:D21">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1210,8 +1245,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E20">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="E4:E21">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1222,8 +1257,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:N20">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="N4:N21">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Added different implementations of RAM + added DU and Critical Timing measurements
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/measurements.xlsx
+++ b/verilog/hardware/processor/source/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759C2A9E-E0D2-9E4C-847F-70429A1694DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1085072A-430A-7D4B-8598-BE4B382A3926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="27000" windowHeight="14240" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>USE_CORRELATING</t>
   </si>
@@ -143,6 +142,24 @@
   </si>
   <si>
     <t>Proposal 2 (proposal 1 + all DSP + 1 word cache)</t>
+  </si>
+  <si>
+    <t>Proposal 1 + Adder + INSRAM1</t>
+  </si>
+  <si>
+    <t>Proposal 2 + INSRAM2</t>
+  </si>
+  <si>
+    <t>Proposal 1 + Adder + INSRAM2</t>
+  </si>
+  <si>
+    <t>Proposal 1 + Adder + INSRAM3</t>
+  </si>
+  <si>
+    <t>Proposal 2 + INSRAM3</t>
+  </si>
+  <si>
+    <t>Proposal 2 + INSRAM1</t>
   </si>
 </sst>
 </file>
@@ -531,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5514D7BD-1B29-5548-99C9-D3A14905CC46}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1253,6 +1270,90 @@
       <c r="I22" s="3">
         <f t="shared" ref="I22" si="4">D22/E22/C$32*1000000000</f>
         <v>2.4639562965549349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N23" s="3">
+        <v>2407</v>
+      </c>
+      <c r="O23" s="3">
+        <v>13.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N24" s="3">
+        <v>2577</v>
+      </c>
+      <c r="O24" s="3">
+        <v>10.93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N25" s="3">
+        <v>2385</v>
+      </c>
+      <c r="O25" s="3">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N26" s="3">
+        <v>2555</v>
+      </c>
+      <c r="O26" s="3">
+        <v>10.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N27" s="3">
+        <v>2385</v>
+      </c>
+      <c r="O27" s="3">
+        <v>13.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2555</v>
+      </c>
+      <c r="O28" s="3">
+        <v>11.1</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added competition DU and critical path measurements
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/measurements.xlsx
+++ b/verilog/hardware/processor/source/measurements.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759C2A9E-E0D2-9E4C-847F-70429A1694DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D911521-B10D-B641-9301-AD31265B2126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="27000" windowHeight="14240" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>USE_CORRELATING</t>
   </si>
@@ -143,6 +142,15 @@
   </si>
   <si>
     <t>Proposal 2 (proposal 1 + all DSP + 1 word cache)</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>Proposal 1  + 1 word cache</t>
+  </si>
+  <si>
+    <t>Proposal 1 + all DSPs</t>
   </si>
 </sst>
 </file>
@@ -204,13 +212,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5514D7BD-1B29-5548-99C9-D3A14905CC46}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -550,31 +561,47 @@
     <col min="11" max="11" width="22" style="3" customWidth="1"/>
     <col min="12" max="14" width="11" style="3"/>
     <col min="15" max="15" width="19.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="17.83203125" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="11" style="3"/>
+    <col min="16" max="17" width="17.83203125" style="3" customWidth="1"/>
+    <col min="18" max="19" width="11" style="4"/>
+    <col min="20" max="22" width="11" style="3"/>
+    <col min="23" max="23" width="18.6640625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="18.33203125" style="3" customWidth="1"/>
+    <col min="25" max="25" width="21" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" s="3"/>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
       <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>32</v>
@@ -616,8 +643,29 @@
       <c r="P2" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -649,8 +697,25 @@
         <f>K4/L4/J$32*1000000000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R4" s="4">
+        <v>6000000</v>
+      </c>
+      <c r="V4" s="3">
+        <v>4632</v>
+      </c>
+      <c r="W4" s="3" t="e">
+        <f>$B4/(U4*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X4" s="3">
+        <v>12.14</v>
+      </c>
+      <c r="Y4" s="3" t="e">
+        <f>T4/U4/R$32*1000000000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -694,8 +759,19 @@
         <f t="shared" ref="P5:P21" si="2">K5/L5/J$32*1000000000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R5" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W5" s="3" t="e">
+        <f>$B5/(U5*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y5" s="3" t="e">
+        <f t="shared" ref="Y5:Y21" si="3">T5/U5/R$32*1000000000</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -727,8 +803,19 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R6" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W6" s="3" t="e">
+        <f>$B6/(U18*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y6" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -760,8 +847,19 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R7" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W7" s="3" t="e">
+        <f>$B7/(U19*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y7" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -786,15 +884,26 @@
         <v>2.023709651645893</v>
       </c>
       <c r="N8" s="3" t="e">
-        <f t="shared" ref="N8:N17" si="3">$B8/(L8*J$32)</f>
+        <f t="shared" ref="N8:N17" si="4">$B8/(L8*J$32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P8" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R8" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W8" s="3" t="e">
+        <f t="shared" ref="W8:W17" si="5">$B8/(U8*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y8" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -819,15 +928,26 @@
         <v>2.0343246779388084</v>
       </c>
       <c r="N9" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P9" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R9" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W9" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y9" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -852,15 +972,26 @@
         <v>2.2026669056724026</v>
       </c>
       <c r="N10" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P10" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R10" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W10" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y10" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -882,15 +1013,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N11" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P11" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R11" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W11" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y11" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
@@ -915,15 +1057,26 @@
         <v>1.929941443594646</v>
       </c>
       <c r="N12" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P12" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R12" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W12" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y12" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -948,15 +1101,26 @@
         <v>2.0572941551202417</v>
       </c>
       <c r="N13" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P13" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R13" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W13" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y13" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -975,15 +1139,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N14" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P14" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R14" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W14" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y14" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1008,15 +1183,26 @@
         <v>4.3402478448275854</v>
       </c>
       <c r="N15" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P15" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R15" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W15" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y15" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1041,15 +1227,26 @@
         <v>749.04214559386992</v>
       </c>
       <c r="N16" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P16" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R16" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W16" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y16" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1068,15 +1265,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N17" s="3" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P17" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R17" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W17" s="3" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y17" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -1123,8 +1331,25 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R18" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="V18" s="3">
+        <v>4677</v>
+      </c>
+      <c r="W18" s="3" t="e">
+        <f>$B18/(#REF!*R$32)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X18" s="3">
+        <v>12.91</v>
+      </c>
+      <c r="Y18" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
@@ -1171,8 +1396,25 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R19" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="V19" s="3">
+        <v>4615</v>
+      </c>
+      <c r="W19" s="3" t="e">
+        <f>$B19/(#REF!*R$32)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X19" s="3">
+        <v>12.01</v>
+      </c>
+      <c r="Y19" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>33</v>
       </c>
@@ -1190,8 +1432,15 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R20" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="Y20" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>34</v>
       </c>
@@ -1226,8 +1475,19 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R21" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="W21" s="3" t="e">
+        <f>$B21/(U21*R$32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y21" s="3" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>35</v>
       </c>
@@ -1251,11 +1511,48 @@
         <v>11.53</v>
       </c>
       <c r="I22" s="3">
-        <f t="shared" ref="I22" si="4">D22/E22/C$32*1000000000</f>
+        <f t="shared" ref="I22" si="6">D22/E22/C$32*1000000000</f>
         <v>2.4639562965549349</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R22" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="V22" s="3">
+        <v>4584</v>
+      </c>
+      <c r="X22" s="3">
+        <v>11.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R23" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="V23" s="3">
+        <v>4826</v>
+      </c>
+      <c r="X23" s="3">
+        <v>11.06</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R24" s="4">
+        <v>12000000</v>
+      </c>
+      <c r="V24" s="3">
+        <v>4406</v>
+      </c>
+      <c r="X24" s="3">
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>22</v>
       </c>
@@ -1299,12 +1596,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:I1"/>
     <mergeCell ref="K1:P1"/>
+    <mergeCell ref="T1:Y1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F22">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1316,7 +1614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G22">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1328,7 +1626,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H22">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1340,7 +1638,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I22">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1352,7 +1650,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D22">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1364,7 +1662,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E22">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1376,6 +1674,138 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N4:N21">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4:K21">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L21">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M21">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O21">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:Q21">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W4:W21">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T4:T21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U21">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V5:V21">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X4:X21">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y4:Y21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1387,55 +1817,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K21">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L21">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M21">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O21">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P21">
+  <conditionalFormatting sqref="V4">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added measurements of morning of competition
</commit_message>
<xml_diff>
--- a/verilog/hardware/processor/source/measurements.xlsx
+++ b/verilog/hardware/processor/source/measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcos/GB3/f-of-e-tools/verilog/hardware/processor/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D911521-B10D-B641-9301-AD31265B2126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4062692-C5D7-B44C-9F05-078B580EAE38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20480" xr2:uid="{3AB65B1E-B0EA-0B4C-85B5-B5A4D7E13C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>USE_CORRELATING</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>Proposal 1 + all DSPs</t>
+  </si>
+  <si>
+    <t>Proposal 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cache 1w 1c init </t>
+  </si>
+  <si>
+    <t>Cache 4w delayed</t>
+  </si>
+  <si>
+    <t>Comp</t>
   </si>
 </sst>
 </file>
@@ -212,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -225,6 +237,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5514D7BD-1B29-5548-99C9-D3A14905CC46}">
   <dimension ref="A1:Y44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1550,6 +1563,38 @@
       </c>
       <c r="X24" s="3">
         <v>14.28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2.1749669999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.000349E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="8">
+        <v>1.170236E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="3">
+        <v>6.1450599999999999E-3</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>